<commit_message>
Test Bayes Classification with different EWMA 01 02 03 04 05 etc
</commit_message>
<xml_diff>
--- a/BayesClassification/results/det_int_0_EWMA_02.xlsx
+++ b/BayesClassification/results/det_int_0_EWMA_02.xlsx
@@ -34,268 +34,268 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">2018-07-31 10:26:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:26:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:26:18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:26:28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:26:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:26:51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:27:02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:27:11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:27:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:27:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:27:47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:27:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:28:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:28:21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:28:32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:28:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:28:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:29:08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:29:21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:29:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:29:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:29:54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:30:04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:30:12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:30:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:30:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:30:41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:30:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:31:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:31:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:31:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:31:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:31:40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:31:48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:32:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:32:09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:32:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:32:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:32:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:32:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:32:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:33:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:33:18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:33:29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:33:37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:33:49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:34:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:34:09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:34:24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:34:37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:34:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:34:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:35:09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:35:21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:35:34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:35:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:35:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:36:08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:36:18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:36:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:36:42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:36:52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:37:08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:37:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:37:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:37:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:37:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:37:57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:38:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:38:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:38:28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:38:34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:38:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:38:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:39:04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:39:14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:39:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:39:32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:39:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:39:54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:40:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:40:15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:40:23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:40:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:40:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:40:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:41:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-07-31 10:41:15</t>
+    <t xml:space="preserve">2018-07-31 14:53:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:53:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:53:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:53:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:54:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:54:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:54:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:54:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:54:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:54:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:55:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:55:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:55:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:55:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:55:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:56:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:56:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:56:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:56:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:56:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:56:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:56:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:57:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:57:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:57:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:57:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:57:42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:57:49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:58:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:58:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:58:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:58:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:58:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:58:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:59:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:59:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:59:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:59:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:59:42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 14:59:52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:00:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:00:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:00:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:00:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:00:37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:00:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:00:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:01:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:01:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:01:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:01:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:01:54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:02:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:02:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:02:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:02:32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:02:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:02:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:03:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:03:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:03:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:03:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:03:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:03:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:04:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:04:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:04:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:04:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:04:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:04:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:05:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:05:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:05:32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:05:42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:05:54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:06:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:06:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:06:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:06:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:06:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:06:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:07:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:07:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:07:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:07:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:07:47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:07:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-31 15:08:09</t>
   </si>
 </sst>
 </file>
@@ -398,8 +398,8 @@
   </sheetPr>
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -430,10 +430,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -444,10 +444,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -458,10 +458,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -472,10 +472,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -486,10 +486,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -640,10 +640,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
@@ -654,10 +654,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>20</v>
@@ -668,10 +668,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>21</v>
@@ -682,10 +682,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>22</v>
@@ -696,10 +696,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>23</v>
@@ -710,10 +710,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>24</v>
@@ -724,10 +724,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>25</v>
@@ -738,10 +738,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>26</v>
@@ -752,10 +752,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>27</v>
@@ -766,10 +766,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>28</v>
@@ -780,10 +780,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>29</v>
@@ -794,10 +794,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>30</v>
@@ -808,10 +808,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>31</v>
@@ -822,10 +822,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>32</v>
@@ -836,10 +836,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>33</v>
@@ -864,10 +864,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>35</v>
@@ -948,10 +948,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>41</v>
@@ -962,10 +962,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>42</v>
@@ -976,10 +976,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>43</v>
@@ -990,10 +990,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>44</v>
@@ -1004,10 +1004,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>45</v>
@@ -1102,10 +1102,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>52</v>
@@ -1116,10 +1116,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>53</v>
@@ -1130,10 +1130,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>54</v>
@@ -1144,10 +1144,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>55</v>
@@ -1158,10 +1158,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>56</v>
@@ -1172,10 +1172,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>57</v>
@@ -1494,10 +1494,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>80</v>
@@ -1536,10 +1536,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>83</v>
@@ -1550,10 +1550,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>84</v>
@@ -1564,10 +1564,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>85</v>
@@ -1592,10 +1592,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>87</v>
@@ -1620,10 +1620,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>89</v>

</xml_diff>